<commit_message>
pequenos ajustes para estudos posteriores
</commit_message>
<xml_diff>
--- a/Sistemas de controle/Lab6/Motor 6.xlsx
+++ b/Sistemas de controle/Lab6/Motor 6.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Users\20.00387-0\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Users\20.01305-0\Desktop\TrabalhosEmGrupo\Sistemas de controle\Lab6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F0F8FF9-F822-4F93-9E67-07E4A7A1B9FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8310D3-4B5B-4EB1-B2C0-4C14AEAD4917}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{E87C7F1D-C110-4D56-9475-DFFB3FF0141F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="13">
   <si>
     <t>yf</t>
   </si>
@@ -71,7 +71,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -97,7 +97,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,6 +134,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -156,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -171,38 +177,39 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -264,6 +271,103 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>179249</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>9138</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ADBD7AA-2220-46C1-812D-9C5A679927D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="457200" y="4038600"/>
+          <a:ext cx="13809524" cy="3095238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>244929</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>244929</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>136071</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Conector de Seta Reta 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{434AA0D2-2088-4FD4-88B8-198C4971F54D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2354036" y="3320143"/>
+          <a:ext cx="0" cy="707571"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -566,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A06A6D-F448-4E4F-B742-A9E2A568F89B}">
-  <dimension ref="B2:H19"/>
+  <dimension ref="B2:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z22" sqref="Z22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,37 +687,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="17">
+      <c r="B2" s="15">
         <v>0.2</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="10" t="s">
         <v>3</v>
       </c>
       <c r="H3" s="7"/>
@@ -622,21 +726,21 @@
       <c r="B4" s="5">
         <v>1</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>23.91</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>0.39</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="10">
         <f>D4-$B$2</f>
         <v>0.19</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="10">
         <f>(C4)/B4</f>
         <v>23.91</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="11">
         <f>C4*0.632</f>
         <v>15.11112</v>
       </c>
@@ -646,21 +750,21 @@
       <c r="B5" s="5">
         <v>2</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>45.765000000000001</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>0.38</v>
       </c>
-      <c r="E5" s="12">
-        <f t="shared" ref="E5:E13" si="0">D5-$B$2</f>
+      <c r="E5" s="10">
+        <f>D5-$B$2</f>
         <v>0.18</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="10">
         <f>(C5)/B5</f>
         <v>22.8825</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="11">
         <f>C5*0.632</f>
         <v>28.923480000000001</v>
       </c>
@@ -670,22 +774,22 @@
       <c r="B6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>70.612200000000001</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>0.37</v>
       </c>
-      <c r="E6" s="12">
-        <f t="shared" si="0"/>
+      <c r="E6" s="10">
+        <f t="shared" ref="E5:E13" si="0">D6-$B$2</f>
         <v>0.16999999999999998</v>
       </c>
-      <c r="F6" s="12">
-        <f t="shared" ref="F6:F13" si="1">(C6)/B6</f>
+      <c r="F6" s="10">
+        <f>(C6)/B6</f>
         <v>23.537400000000002</v>
       </c>
-      <c r="G6" s="13">
-        <f t="shared" ref="G6:G13" si="2">C6*0.632</f>
+      <c r="G6" s="11">
+        <f t="shared" ref="G6:G13" si="1">C6*0.632</f>
         <v>44.6269104</v>
       </c>
       <c r="H6" s="7"/>
@@ -694,22 +798,22 @@
       <c r="B7" s="5">
         <v>4</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>94.997200000000007</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>0.36</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="10">
         <f t="shared" si="0"/>
         <v>0.15999999999999998</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="10">
+        <f t="shared" ref="F6:F13" si="2">(C7)/B7</f>
+        <v>23.749300000000002</v>
+      </c>
+      <c r="G7" s="11">
         <f t="shared" si="1"/>
-        <v>23.749300000000002</v>
-      </c>
-      <c r="G7" s="13">
-        <f t="shared" si="2"/>
         <v>60.038230400000003</v>
       </c>
       <c r="H7" s="7"/>
@@ -718,22 +822,22 @@
       <c r="B8" s="5">
         <v>5</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <v>119.455</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>0.36</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="10">
         <f t="shared" si="0"/>
         <v>0.15999999999999998</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="10">
         <f>(C8)/B8</f>
         <v>23.890999999999998</v>
       </c>
-      <c r="G8" s="13">
-        <f t="shared" si="2"/>
+      <c r="G8" s="11">
+        <f t="shared" si="1"/>
         <v>75.495559999999998</v>
       </c>
       <c r="H8" s="7"/>
@@ -742,22 +846,22 @@
       <c r="B9" s="5">
         <v>6</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <v>144.44399999999999</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>0.36</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="10">
         <f t="shared" si="0"/>
         <v>0.15999999999999998</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="10">
+        <f t="shared" si="2"/>
+        <v>24.073999999999998</v>
+      </c>
+      <c r="G9" s="11">
         <f t="shared" si="1"/>
-        <v>24.073999999999998</v>
-      </c>
-      <c r="G9" s="13">
-        <f t="shared" si="2"/>
         <v>91.288607999999996</v>
       </c>
       <c r="H9" s="7"/>
@@ -766,22 +870,22 @@
       <c r="B10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <v>166.499</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>0.35</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="10">
         <f t="shared" si="0"/>
         <v>0.14999999999999997</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="11">
+        <f t="shared" si="2"/>
+        <v>23.785571428571426</v>
+      </c>
+      <c r="G10" s="11">
         <f t="shared" si="1"/>
-        <v>23.785571428571426</v>
-      </c>
-      <c r="G10" s="13">
-        <f t="shared" si="2"/>
         <v>105.227368</v>
       </c>
       <c r="H10" s="7"/>
@@ -790,22 +894,22 @@
       <c r="B11" s="5">
         <v>8</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="9">
         <v>191.13</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>0.35</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="10">
         <f t="shared" si="0"/>
         <v>0.14999999999999997</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="10">
+        <f t="shared" si="2"/>
+        <v>23.891249999999999</v>
+      </c>
+      <c r="G11" s="11">
         <f t="shared" si="1"/>
-        <v>23.891249999999999</v>
-      </c>
-      <c r="G11" s="13">
-        <f t="shared" si="2"/>
         <v>120.79416000000001</v>
       </c>
       <c r="H11" s="7"/>
@@ -814,22 +918,22 @@
       <c r="B12" s="5">
         <v>9</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <v>217.32300000000001</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <v>0.35</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="10">
         <f t="shared" si="0"/>
         <v>0.14999999999999997</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="10">
+        <f t="shared" si="2"/>
+        <v>24.147000000000002</v>
+      </c>
+      <c r="G12" s="11">
         <f t="shared" si="1"/>
-        <v>24.147000000000002</v>
-      </c>
-      <c r="G12" s="13">
-        <f t="shared" si="2"/>
         <v>137.34813600000001</v>
       </c>
       <c r="H12" s="7"/>
@@ -838,44 +942,44 @@
       <c r="B13" s="5">
         <v>10</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <v>241.24199999999999</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>0.35</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="10">
         <f t="shared" si="0"/>
         <v>0.14999999999999997</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="10">
+        <f t="shared" si="2"/>
+        <v>24.124199999999998</v>
+      </c>
+      <c r="G13" s="11">
         <f t="shared" si="1"/>
-        <v>24.124199999999998</v>
-      </c>
-      <c r="G13" s="13">
-        <f t="shared" si="2"/>
         <v>152.464944</v>
       </c>
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="15">
+      <c r="C14" s="12"/>
+      <c r="D14" s="13">
         <f>AVERAGE(D4:D13)</f>
         <v>0.36199999999999999</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="13">
         <f>AVERAGE(E4:E13)</f>
         <v>0.16199999999999995</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="14">
         <f>AVERAGE(F4:F13)</f>
         <v>23.79922214285714</v>
       </c>
-      <c r="G14" s="14"/>
+      <c r="G14" s="12"/>
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -914,10 +1018,26 @@
       </c>
     </row>
     <row r="18" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
       <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>